<commit_message>
Removed test template files, updated sync script to support local HTTPS development
</commit_message>
<xml_diff>
--- a/CustomField_LookupTable.xlsx
+++ b/CustomField_LookupTable.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29628"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29725"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://netorgft5071812-my.sharepoint.com/personal/tdolan_quillarrowlaw_com/Documents/Documents/ClioTemplates_CustomFields_MassUpdate/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="254" documentId="8_{E80BBBE6-58B7-4864-BD78-E0E1CDA502EC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{C1C4EF82-F195-4B25-9DF3-03B687033B96}"/>
+  <xr:revisionPtr revIDLastSave="268" documentId="8_{E80BBBE6-58B7-4864-BD78-E0E1CDA502EC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{88F9609E-8F7B-4273-AD1B-688003CE4F5F}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{28124E9B-F57B-404E-A792-64830DDEDE95}"/>
+    <workbookView xWindow="30735" yWindow="1035" windowWidth="27000" windowHeight="14115" xr2:uid="{28124E9B-F57B-404E-A792-64830DDEDE95}"/>
   </bookViews>
   <sheets>
     <sheet name="LookupTable" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="8">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
   <si>
     <t>New_Value</t>
   </si>
@@ -44,22 +44,16 @@
     <t>Old_Value</t>
   </si>
   <si>
-    <t>&lt;&lt; Matter.ResponsibleAttorney &gt;&gt;</t>
-  </si>
-  <si>
-    <t>&lt;&lt; MATTER.CUSTOMFIELD.PLAINTIFFSNAMESHORT &gt;&gt;</t>
-  </si>
-  <si>
-    <t>&lt;&lt; Matter.CustomField.PlaintiffsFullLegalName &gt;&gt;</t>
-  </si>
-  <si>
-    <t>&lt;&lt; Matter.ResponsibleAttorney_CHANGE1 &gt;&gt;</t>
-  </si>
-  <si>
     <t>&lt;&lt; MATTER.CUSTOMFIELD.PLAINTIFFSNAMESHORT_CHANGE2 &gt;&gt;</t>
   </si>
   <si>
-    <t>&lt;&lt; Matter.CustomField.PlaintiffsFullLegalName_CHANGE3 &gt;&gt;</t>
+    <t>&lt;&lt;Matter.CustomField.PlaintiffsFullLegalName_CHANGE1 &gt;&gt;</t>
+  </si>
+  <si>
+    <t>&lt;&lt;Matter.CustomField.PlaintiffsFullLegalName &gt;&gt;</t>
+  </si>
+  <si>
+    <t>&lt;&lt;MATTER.CUSTOMFIELD.PLAINTIFFSNAMESHORT&gt;&gt;</t>
   </si>
 </sst>
 </file>
@@ -91,7 +85,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="3">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -112,26 +106,11 @@
       <bottom/>
       <diagonal/>
     </border>
-    <border>
-      <left style="medium">
-        <color indexed="64"/>
-      </left>
-      <right style="medium">
-        <color indexed="64"/>
-      </right>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -140,9 +119,6 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -185,8 +161,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{6CDBC208-8FF6-478D-95B6-188E225F38B1}" name="Table1" displayName="Table1" ref="A1:B9" totalsRowShown="0" headerRowDxfId="0">
-  <autoFilter ref="A1:B9" xr:uid="{6CDBC208-8FF6-478D-95B6-188E225F38B1}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{6CDBC208-8FF6-478D-95B6-188E225F38B1}" name="Table1" displayName="Table1" ref="A1:B3" totalsRowShown="0" headerRowDxfId="0">
+  <autoFilter ref="A1:B3" xr:uid="{6CDBC208-8FF6-478D-95B6-188E225F38B1}"/>
   <tableColumns count="2">
     <tableColumn id="1" xr3:uid="{52BB13A1-40AB-4518-B0DE-62637CB7D74A}" name="Old_Value"/>
     <tableColumn id="2" xr3:uid="{06BCDB60-C4F4-4E5F-B692-5B8737E55DE6}" name="New_Value"/>
@@ -512,10 +488,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AAF23435-C8D7-4BEB-89A9-D8A938A40D38}">
-  <dimension ref="A1:B9"/>
+  <dimension ref="A1:B3"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B14" sqref="B14"/>
+      <selection activeCell="B8" sqref="B8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -534,66 +510,18 @@
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" s="3" t="s">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A3" s="4" t="s">
-        <v>3</v>
-      </c>
-      <c r="B3" s="4" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A4" s="4" t="s">
-        <v>4</v>
-      </c>
-      <c r="B4" s="4" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A5" s="4" t="s">
-        <v>2</v>
-      </c>
-      <c r="B5" s="4" t="s">
+      <c r="A3" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A6" s="4" t="s">
-        <v>3</v>
-      </c>
-      <c r="B6" s="4" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A7" s="4" t="s">
-        <v>4</v>
-      </c>
-      <c r="B7" s="4" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A8" t="s">
-        <v>3</v>
-      </c>
-      <c r="B8" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A9" t="s">
-        <v>4</v>
-      </c>
-      <c r="B9" t="s">
-        <v>7</v>
+      <c r="B3" t="s">
+        <v>2</v>
       </c>
     </row>
   </sheetData>

</xml_diff>